<commit_message>
feat: create Name and Team Name columns to add data
</commit_message>
<xml_diff>
--- a/name_list.xlsx
+++ b/name_list.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\certificates_generation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B33A1E-1358-49CC-9AD7-57D9D7A8502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +24,42 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>John joe</t>
+  </si>
+  <si>
+    <t>Team 01</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +369,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: add data to excel sheet
</commit_message>
<xml_diff>
--- a/name_list.xlsx
+++ b/name_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\certificates_generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B33A1E-1358-49CC-9AD7-57D9D7A8502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DED8E5-4E58-487E-BD52-A009559E04E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -33,17 +33,29 @@
     <t>Team Name</t>
   </si>
   <si>
-    <t>John joe</t>
-  </si>
-  <si>
     <t>Team 01</t>
+  </si>
+  <si>
+    <t>Sarah Lee</t>
+  </si>
+  <si>
+    <t>David Smith</t>
+  </si>
+  <si>
+    <t>Emily Clark</t>
+  </si>
+  <si>
+    <t>Team 02</t>
+  </si>
+  <si>
+    <t>Team 03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,14 +64,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -74,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -82,14 +100,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,38 +491,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: remove team column
</commit_message>
<xml_diff>
--- a/name_list.xlsx
+++ b/name_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\certificates_generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DED8E5-4E58-487E-BD52-A009559E04E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E873B653-CAA1-43C6-840A-7B39998E4CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>Team 01</t>
   </si>
   <si>
     <t>Sarah Lee</t>
@@ -43,12 +37,6 @@
   </si>
   <si>
     <t>Emily Clark</t>
-  </si>
-  <si>
-    <t>Team 02</t>
-  </si>
-  <si>
-    <t>Team 03</t>
   </si>
 </sst>
 </file>
@@ -92,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,63 +107,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -200,17 +131,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,56 +423,48 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
+      <c r="A4" s="4" t="s">
+        <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>

</xml_diff>